<commit_message>
Fixed the UI and added expenses window.
</commit_message>
<xml_diff>
--- a/expenses.xlsx
+++ b/expenses.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,6 +486,44 @@
       </c>
       <c r="E3" t="inlineStr"/>
     </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Food</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>500</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>July 10, 2026</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Transport</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1111</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>May 18 2025</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added bills and debt windows.
</commit_message>
<xml_diff>
--- a/expenses.xlsx
+++ b/expenses.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -524,6 +524,63 @@
       </c>
       <c r="E5" t="inlineStr"/>
     </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Food</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>120</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>10-31-2025</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Water</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>11-01-2025</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Water</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>11-01-2025</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>